<commit_message>
feat: Add new feature, plotting out the attention map for image
</commit_message>
<xml_diff>
--- a/notebooks/data.xlsx
+++ b/notebooks/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H189"/>
+  <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>low uncertainty</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>label</t>
         </is>
       </c>
@@ -495,6 +500,9 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -519,6 +527,9 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -545,6 +556,9 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -573,6 +587,9 @@
       <c r="H5" t="n">
         <v>1</v>
       </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -597,6 +614,9 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -625,6 +645,9 @@
       <c r="H7" t="n">
         <v>1</v>
       </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -651,6 +674,9 @@
       <c r="H8" t="n">
         <v>1</v>
       </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -677,6 +703,9 @@
       <c r="H9" t="n">
         <v>1</v>
       </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -701,6 +730,9 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -729,6 +761,9 @@
       <c r="H11" t="n">
         <v>1</v>
       </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -753,6 +788,9 @@
         <v>1</v>
       </c>
       <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -781,6 +819,9 @@
       <c r="H13" t="n">
         <v>1</v>
       </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -805,6 +846,9 @@
         <v>1</v>
       </c>
       <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -831,6 +875,9 @@
         <v>1</v>
       </c>
       <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -857,6 +904,9 @@
         <v>1</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -883,6 +933,9 @@
         <v>1</v>
       </c>
       <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -911,6 +964,9 @@
       <c r="H18" t="n">
         <v>1</v>
       </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -935,6 +991,9 @@
         <v>1</v>
       </c>
       <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -963,6 +1022,9 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -989,6 +1051,9 @@
       <c r="H21" t="n">
         <v>1</v>
       </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1015,6 +1080,9 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1041,6 +1109,9 @@
       <c r="H23" t="n">
         <v>1</v>
       </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1065,6 +1136,9 @@
         <v>1</v>
       </c>
       <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1091,6 +1165,9 @@
         <v>1</v>
       </c>
       <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1119,6 +1196,9 @@
       <c r="H26" t="n">
         <v>1</v>
       </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1145,6 +1225,9 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1171,6 +1254,9 @@
       <c r="H28" t="n">
         <v>1</v>
       </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1195,6 +1281,9 @@
         <v>1</v>
       </c>
       <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1221,6 +1310,9 @@
         <v>1</v>
       </c>
       <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1249,6 +1341,9 @@
       <c r="H31" t="n">
         <v>1</v>
       </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1273,6 +1368,9 @@
         <v>1</v>
       </c>
       <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1301,6 +1399,9 @@
       <c r="H33" t="n">
         <v>1</v>
       </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1325,6 +1426,9 @@
         <v>1</v>
       </c>
       <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1353,6 +1457,9 @@
       <c r="H35" t="n">
         <v>1</v>
       </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1377,6 +1484,9 @@
         <v>1</v>
       </c>
       <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1403,6 +1513,9 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1431,6 +1544,9 @@
       <c r="H38" t="n">
         <v>1</v>
       </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1457,6 +1573,9 @@
       <c r="H39" t="n">
         <v>0</v>
       </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1481,6 +1600,9 @@
         <v>1</v>
       </c>
       <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1507,6 +1629,9 @@
         <v>1</v>
       </c>
       <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1535,6 +1660,9 @@
       <c r="H42" t="n">
         <v>0</v>
       </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1561,6 +1689,9 @@
       <c r="H43" t="n">
         <v>0</v>
       </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1587,6 +1718,9 @@
       <c r="H44" t="n">
         <v>1</v>
       </c>
+      <c r="I44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1611,6 +1745,9 @@
         <v>1</v>
       </c>
       <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1639,6 +1776,9 @@
       <c r="H46" t="n">
         <v>0</v>
       </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1665,6 +1805,9 @@
       <c r="H47" t="n">
         <v>0</v>
       </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1689,6 +1832,9 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1715,6 +1861,9 @@
         <v>1</v>
       </c>
       <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1741,6 +1890,9 @@
         <v>1</v>
       </c>
       <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1769,6 +1921,9 @@
       <c r="H51" t="n">
         <v>1</v>
       </c>
+      <c r="I51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1795,6 +1950,9 @@
       <c r="H52" t="n">
         <v>0</v>
       </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1819,6 +1977,9 @@
         <v>0</v>
       </c>
       <c r="H53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1845,6 +2006,9 @@
         <v>1</v>
       </c>
       <c r="H54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1873,6 +2037,9 @@
       <c r="H55" t="n">
         <v>0</v>
       </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1899,6 +2066,9 @@
       <c r="H56" t="n">
         <v>1</v>
       </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1923,6 +2093,9 @@
         <v>1</v>
       </c>
       <c r="H57" t="n">
+        <v>1</v>
+      </c>
+      <c r="I57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1951,6 +2124,9 @@
       <c r="H58" t="n">
         <v>1</v>
       </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1975,6 +2151,9 @@
         <v>1</v>
       </c>
       <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2003,6 +2182,9 @@
       <c r="H60" t="n">
         <v>0</v>
       </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2029,6 +2211,9 @@
       <c r="H61" t="n">
         <v>1</v>
       </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2053,6 +2238,9 @@
         <v>1</v>
       </c>
       <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2081,6 +2269,9 @@
       <c r="H63" t="n">
         <v>0</v>
       </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2107,6 +2298,9 @@
       <c r="H64" t="n">
         <v>1</v>
       </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2131,6 +2325,9 @@
         <v>1</v>
       </c>
       <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2157,6 +2354,9 @@
         <v>1</v>
       </c>
       <c r="H66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2185,6 +2385,9 @@
       <c r="H67" t="n">
         <v>1</v>
       </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2211,6 +2414,9 @@
       <c r="H68" t="n">
         <v>1</v>
       </c>
+      <c r="I68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2235,6 +2441,9 @@
         <v>1</v>
       </c>
       <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2261,6 +2470,9 @@
         <v>1</v>
       </c>
       <c r="H70" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2289,6 +2501,9 @@
       <c r="H71" t="n">
         <v>1</v>
       </c>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2313,6 +2528,9 @@
         <v>1</v>
       </c>
       <c r="H72" t="n">
+        <v>1</v>
+      </c>
+      <c r="I72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2339,6 +2557,9 @@
         <v>1</v>
       </c>
       <c r="H73" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2367,6 +2588,9 @@
       <c r="H74" t="n">
         <v>0</v>
       </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2391,6 +2615,9 @@
         <v>1</v>
       </c>
       <c r="H75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2417,6 +2644,9 @@
         <v>1</v>
       </c>
       <c r="H76" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2445,6 +2675,9 @@
       <c r="H77" t="n">
         <v>0</v>
       </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2469,6 +2702,9 @@
         <v>1</v>
       </c>
       <c r="H78" t="n">
+        <v>1</v>
+      </c>
+      <c r="I78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2495,6 +2731,9 @@
         <v>1</v>
       </c>
       <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2521,6 +2760,9 @@
         <v>1</v>
       </c>
       <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2547,6 +2789,9 @@
         <v>1</v>
       </c>
       <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2573,6 +2818,9 @@
         <v>1</v>
       </c>
       <c r="H82" t="n">
+        <v>1</v>
+      </c>
+      <c r="I82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2601,6 +2849,9 @@
       <c r="H83" t="n">
         <v>1</v>
       </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2627,6 +2878,9 @@
       <c r="H84" t="n">
         <v>1</v>
       </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2653,6 +2907,9 @@
       <c r="H85" t="n">
         <v>1</v>
       </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2677,6 +2934,9 @@
         <v>0</v>
       </c>
       <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2705,6 +2965,9 @@
       <c r="H87" t="n">
         <v>1</v>
       </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2731,6 +2994,9 @@
       <c r="H88" t="n">
         <v>1</v>
       </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2757,6 +3023,9 @@
       <c r="H89" t="n">
         <v>1</v>
       </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2781,6 +3050,9 @@
         <v>1</v>
       </c>
       <c r="H90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2807,6 +3079,9 @@
         <v>1</v>
       </c>
       <c r="H91" t="n">
+        <v>1</v>
+      </c>
+      <c r="I91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2833,6 +3108,9 @@
         <v>1</v>
       </c>
       <c r="H92" t="n">
+        <v>1</v>
+      </c>
+      <c r="I92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2859,6 +3137,9 @@
         <v>1</v>
       </c>
       <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2887,6 +3168,9 @@
       <c r="H94" t="n">
         <v>0</v>
       </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2913,6 +3197,9 @@
       <c r="H95" t="n">
         <v>1</v>
       </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2937,6 +3224,9 @@
         <v>1</v>
       </c>
       <c r="H96" t="n">
+        <v>1</v>
+      </c>
+      <c r="I96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2963,6 +3253,9 @@
         <v>1</v>
       </c>
       <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2989,6 +3282,9 @@
         <v>1</v>
       </c>
       <c r="H98" t="n">
+        <v>1</v>
+      </c>
+      <c r="I98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3017,6 +3313,9 @@
       <c r="H99" t="n">
         <v>1</v>
       </c>
+      <c r="I99" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3041,6 +3340,9 @@
         <v>1</v>
       </c>
       <c r="H100" t="n">
+        <v>1</v>
+      </c>
+      <c r="I100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3067,6 +3369,9 @@
         <v>1</v>
       </c>
       <c r="H101" t="n">
+        <v>1</v>
+      </c>
+      <c r="I101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3095,6 +3400,9 @@
       <c r="H102" t="n">
         <v>0</v>
       </c>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3121,6 +3429,9 @@
       <c r="H103" t="n">
         <v>1</v>
       </c>
+      <c r="I103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3147,6 +3458,9 @@
       <c r="H104" t="n">
         <v>1</v>
       </c>
+      <c r="I104" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3173,6 +3487,9 @@
       <c r="H105" t="n">
         <v>1</v>
       </c>
+      <c r="I105" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -3197,6 +3514,9 @@
         <v>1</v>
       </c>
       <c r="H106" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3225,6 +3545,9 @@
       <c r="H107" t="n">
         <v>1</v>
       </c>
+      <c r="I107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3249,6 +3572,9 @@
         <v>0</v>
       </c>
       <c r="H108" t="n">
+        <v>1</v>
+      </c>
+      <c r="I108" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3277,6 +3603,9 @@
       <c r="H109" t="n">
         <v>0</v>
       </c>
+      <c r="I109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3303,6 +3632,9 @@
       <c r="H110" t="n">
         <v>1</v>
       </c>
+      <c r="I110" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3327,6 +3659,9 @@
         <v>1</v>
       </c>
       <c r="H111" t="n">
+        <v>1</v>
+      </c>
+      <c r="I111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3353,6 +3688,9 @@
         <v>0</v>
       </c>
       <c r="H112" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3379,6 +3717,9 @@
         <v>1</v>
       </c>
       <c r="H113" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3405,6 +3746,9 @@
         <v>0</v>
       </c>
       <c r="H114" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3431,6 +3775,9 @@
         <v>0</v>
       </c>
       <c r="H115" t="n">
+        <v>1</v>
+      </c>
+      <c r="I115" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3457,6 +3804,9 @@
         <v>0</v>
       </c>
       <c r="H116" t="n">
+        <v>1</v>
+      </c>
+      <c r="I116" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3483,6 +3833,9 @@
         <v>0</v>
       </c>
       <c r="H117" t="n">
+        <v>1</v>
+      </c>
+      <c r="I117" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3509,6 +3862,9 @@
         <v>1</v>
       </c>
       <c r="H118" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3535,6 +3891,9 @@
         <v>0</v>
       </c>
       <c r="H119" t="n">
+        <v>1</v>
+      </c>
+      <c r="I119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3561,6 +3920,9 @@
         <v>0</v>
       </c>
       <c r="H120" t="n">
+        <v>1</v>
+      </c>
+      <c r="I120" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3587,6 +3949,9 @@
         <v>1</v>
       </c>
       <c r="H121" t="n">
+        <v>1</v>
+      </c>
+      <c r="I121" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3613,6 +3978,9 @@
         <v>0</v>
       </c>
       <c r="H122" t="n">
+        <v>1</v>
+      </c>
+      <c r="I122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3639,6 +4007,9 @@
         <v>0</v>
       </c>
       <c r="H123" t="n">
+        <v>1</v>
+      </c>
+      <c r="I123" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3665,6 +4036,9 @@
         <v>0</v>
       </c>
       <c r="H124" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3691,6 +4065,9 @@
         <v>0</v>
       </c>
       <c r="H125" t="n">
+        <v>1</v>
+      </c>
+      <c r="I125" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3717,6 +4094,9 @@
         <v>1</v>
       </c>
       <c r="H126" t="n">
+        <v>1</v>
+      </c>
+      <c r="I126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3743,6 +4123,9 @@
         <v>0</v>
       </c>
       <c r="H127" t="n">
+        <v>1</v>
+      </c>
+      <c r="I127" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3769,6 +4152,9 @@
         <v>1</v>
       </c>
       <c r="H128" t="n">
+        <v>1</v>
+      </c>
+      <c r="I128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3795,6 +4181,9 @@
         <v>1</v>
       </c>
       <c r="H129" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3821,6 +4210,9 @@
         <v>1</v>
       </c>
       <c r="H130" t="n">
+        <v>1</v>
+      </c>
+      <c r="I130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3849,6 +4241,9 @@
       <c r="H131" t="n">
         <v>1</v>
       </c>
+      <c r="I131" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -3873,6 +4268,9 @@
         <v>0</v>
       </c>
       <c r="H132" t="n">
+        <v>1</v>
+      </c>
+      <c r="I132" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3901,6 +4299,9 @@
       <c r="H133" t="n">
         <v>1</v>
       </c>
+      <c r="I133" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -3925,6 +4326,9 @@
         <v>1</v>
       </c>
       <c r="H134" t="n">
+        <v>1</v>
+      </c>
+      <c r="I134" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3953,6 +4357,9 @@
       <c r="H135" t="n">
         <v>0</v>
       </c>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -3977,6 +4384,9 @@
         <v>1</v>
       </c>
       <c r="H136" t="n">
+        <v>1</v>
+      </c>
+      <c r="I136" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4003,6 +4413,9 @@
         <v>1</v>
       </c>
       <c r="H137" t="n">
+        <v>1</v>
+      </c>
+      <c r="I137" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4029,6 +4442,9 @@
         <v>0</v>
       </c>
       <c r="H138" t="n">
+        <v>1</v>
+      </c>
+      <c r="I138" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4055,6 +4471,9 @@
         <v>0</v>
       </c>
       <c r="H139" t="n">
+        <v>1</v>
+      </c>
+      <c r="I139" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4083,6 +4502,9 @@
       <c r="H140" t="n">
         <v>1</v>
       </c>
+      <c r="I140" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -4107,6 +4529,9 @@
         <v>1</v>
       </c>
       <c r="H141" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4133,6 +4558,9 @@
         <v>1</v>
       </c>
       <c r="H142" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4159,6 +4587,9 @@
         <v>1</v>
       </c>
       <c r="H143" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4185,6 +4616,9 @@
         <v>1</v>
       </c>
       <c r="H144" t="n">
+        <v>1</v>
+      </c>
+      <c r="I144" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4213,6 +4647,9 @@
       <c r="H145" t="n">
         <v>0</v>
       </c>
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4239,6 +4676,9 @@
       <c r="H146" t="n">
         <v>0</v>
       </c>
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -4263,6 +4703,9 @@
         <v>1</v>
       </c>
       <c r="H147" t="n">
+        <v>1</v>
+      </c>
+      <c r="I147" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4289,6 +4732,9 @@
         <v>1</v>
       </c>
       <c r="H148" t="n">
+        <v>1</v>
+      </c>
+      <c r="I148" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4315,6 +4761,9 @@
         <v>1</v>
       </c>
       <c r="H149" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4341,6 +4790,9 @@
         <v>1</v>
       </c>
       <c r="H150" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4369,6 +4821,9 @@
       <c r="H151" t="n">
         <v>0</v>
       </c>
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -4393,6 +4848,9 @@
         <v>1</v>
       </c>
       <c r="H152" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4421,6 +4879,9 @@
       <c r="H153" t="n">
         <v>0</v>
       </c>
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -4445,6 +4906,9 @@
         <v>1</v>
       </c>
       <c r="H154" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4471,6 +4935,9 @@
         <v>1</v>
       </c>
       <c r="H155" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4499,6 +4966,9 @@
       <c r="H156" t="n">
         <v>0</v>
       </c>
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -4525,6 +4995,9 @@
       <c r="H157" t="n">
         <v>0</v>
       </c>
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -4549,6 +5022,9 @@
         <v>1</v>
       </c>
       <c r="H158" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4575,6 +5051,9 @@
         <v>1</v>
       </c>
       <c r="H159" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4601,6 +5080,9 @@
         <v>1</v>
       </c>
       <c r="H160" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4627,6 +5109,9 @@
         <v>1</v>
       </c>
       <c r="H161" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4653,6 +5138,9 @@
         <v>1</v>
       </c>
       <c r="H162" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4679,6 +5167,9 @@
         <v>1</v>
       </c>
       <c r="H163" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4705,6 +5196,9 @@
         <v>1</v>
       </c>
       <c r="H164" t="n">
+        <v>0</v>
+      </c>
+      <c r="I164" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4731,6 +5225,9 @@
         <v>1</v>
       </c>
       <c r="H165" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4757,6 +5254,9 @@
         <v>1</v>
       </c>
       <c r="H166" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4783,6 +5283,9 @@
         <v>1</v>
       </c>
       <c r="H167" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4809,6 +5312,9 @@
         <v>1</v>
       </c>
       <c r="H168" t="n">
+        <v>0</v>
+      </c>
+      <c r="I168" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4837,6 +5343,9 @@
       <c r="H169" t="n">
         <v>1</v>
       </c>
+      <c r="I169" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -4863,6 +5372,9 @@
       <c r="H170" t="n">
         <v>0</v>
       </c>
+      <c r="I170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -4887,6 +5399,9 @@
         <v>1</v>
       </c>
       <c r="H171" t="n">
+        <v>1</v>
+      </c>
+      <c r="I171" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4913,6 +5428,9 @@
         <v>1</v>
       </c>
       <c r="H172" t="n">
+        <v>1</v>
+      </c>
+      <c r="I172" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4939,6 +5457,9 @@
         <v>1</v>
       </c>
       <c r="H173" t="n">
+        <v>1</v>
+      </c>
+      <c r="I173" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4967,6 +5488,9 @@
       <c r="H174" t="n">
         <v>0</v>
       </c>
+      <c r="I174" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -4993,6 +5517,9 @@
       <c r="H175" t="n">
         <v>1</v>
       </c>
+      <c r="I175" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -5019,6 +5546,9 @@
       <c r="H176" t="n">
         <v>0</v>
       </c>
+      <c r="I176" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -5045,6 +5575,9 @@
       <c r="H177" t="n">
         <v>0</v>
       </c>
+      <c r="I177" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -5069,6 +5602,9 @@
         <v>1</v>
       </c>
       <c r="H178" t="n">
+        <v>1</v>
+      </c>
+      <c r="I178" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5095,6 +5631,9 @@
         <v>1</v>
       </c>
       <c r="H179" t="n">
+        <v>0</v>
+      </c>
+      <c r="I179" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5123,6 +5662,9 @@
       <c r="H180" t="n">
         <v>1</v>
       </c>
+      <c r="I180" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -5147,6 +5689,9 @@
         <v>1</v>
       </c>
       <c r="H181" t="n">
+        <v>1</v>
+      </c>
+      <c r="I181" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5173,6 +5718,9 @@
         <v>1</v>
       </c>
       <c r="H182" t="n">
+        <v>1</v>
+      </c>
+      <c r="I182" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5201,6 +5749,9 @@
       <c r="H183" t="n">
         <v>0</v>
       </c>
+      <c r="I183" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -5227,6 +5778,9 @@
       <c r="H184" t="n">
         <v>0</v>
       </c>
+      <c r="I184" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -5251,6 +5805,9 @@
         <v>1</v>
       </c>
       <c r="H185" t="n">
+        <v>0</v>
+      </c>
+      <c r="I185" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5279,6 +5836,9 @@
       <c r="H186" t="n">
         <v>0</v>
       </c>
+      <c r="I186" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -5303,6 +5863,9 @@
         <v>1</v>
       </c>
       <c r="H187" t="n">
+        <v>0</v>
+      </c>
+      <c r="I187" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5331,6 +5894,9 @@
       <c r="H188" t="n">
         <v>1</v>
       </c>
+      <c r="I188" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -5355,6 +5921,9 @@
         <v>1</v>
       </c>
       <c r="H189" t="n">
+        <v>0</v>
+      </c>
+      <c r="I189" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>